<commit_message>
Temp Screening, Visitor Purpose Related Questions, Updates Screening Questionnaire
</commit_message>
<xml_diff>
--- a/documentation/Development Task list.xlsx
+++ b/documentation/Development Task list.xlsx
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,16 +1095,16 @@
       <c r="G9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>9</v>
+      <c r="H9" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I9" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J9" s="13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>C</v>
       </c>
       <c r="K9" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1195,16 +1195,16 @@
       <c r="G11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="14" t="s">
-        <v>9</v>
+      <c r="H11" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I11" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J11" s="13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>C</v>
       </c>
       <c r="K11" s="13" t="str">
         <f t="shared" si="2"/>
@@ -1245,16 +1245,16 @@
       <c r="G12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>9</v>
+      <c r="H12" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I12" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>C</v>
       </c>
       <c r="K12" s="13" t="str">
         <f t="shared" si="2"/>

</xml_diff>